<commit_message>
Working MPI Linear Regression
MPI Linear Regression now working and updated the journal and times document
</commit_message>
<xml_diff>
--- a/Linear Regression TImes.xlsx
+++ b/Linear Regression TImes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harpr\Desktop\HPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9A524100-BABE-4571-A863-C1FFBB560985}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{365C1A7A-759B-4ACD-93A4-A794A417D2B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20554" windowHeight="7269" xr2:uid="{0050925B-5CB7-4C60-A950-D7FE4F2B9457}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Run</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t>MPI (print status)</t>
   </si>
 </sst>
 </file>
@@ -229,10 +232,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -566,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D219EAB3-40B1-40D8-895F-FF3FECA27EF5}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -577,151 +579,211 @@
     <col min="1" max="1" width="5.53515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.53515625" customWidth="1"/>
-    <col min="5" max="5" width="7.15234375" customWidth="1"/>
+    <col min="4" max="4" width="15.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0.13223399999999999</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="4">
+      <c r="C2" s="2"/>
+      <c r="D2">
+        <v>0.79990604899999995</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.38097101999999999</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>0.13209399999999999</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="4">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>0.79816991900000001</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.37170944299999997</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.13380900000000001</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="4">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.79621488399999996</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.365996563</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>0.13314899999999999</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>0.79451043899999996</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.36351255599999999</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>0.13206000000000001</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="4">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>0.79235682600000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.37894454300000002</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>0.132188</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="4">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0.79005882000000005</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.37701122799999998</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>0.131693</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="4">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>0.78543482399999998</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.375015072</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>0.13173799999999999</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="4">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>0.80184527800000005</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.36816629400000001</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>0.13134999999999999</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="4">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>0.13255600000000001</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1">
         <f>AVERAGE(B2:B11)</f>
         <v>0.13228710000000002</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+      <c r="C12" s="4" t="e">
+        <f>AVERAGE(C2:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" ref="D12:F12" si="0">AVERAGE(D2:D11)</f>
+        <v>0.79481212987500005</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.37266583987499996</v>
+      </c>
+      <c r="F12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>